<commit_message>
Update 14-16 all_dmu analysis.xlsx
</commit_message>
<xml_diff>
--- a/14-16 all_dmu analysis.xlsx
+++ b/14-16 all_dmu analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tungwu/Documents/GitHub/insurer-emperical-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E87695-C0DF-3E42-A801-67D372BB46DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89EFC1B-DBF1-E941-BDC6-1038F565A0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,496 +55,498 @@
     <t>operation_exp cosine similarity</t>
   </si>
   <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Efficiency Change</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>AIA Taiwan 14</t>
+  </si>
+  <si>
+    <t>AIA Taiwan 15</t>
+  </si>
+  <si>
+    <t>AIA Taiwan 16</t>
+  </si>
+  <si>
+    <t>Allianz Taiwan Life 14</t>
+  </si>
+  <si>
+    <t>Allianz Taiwan Life 15</t>
+  </si>
+  <si>
+    <t>Allianz Taiwan Life 16</t>
+  </si>
+  <si>
+    <t>Bank Taiwan Life 14</t>
+  </si>
+  <si>
+    <t>Bank Taiwan Life 15</t>
+  </si>
+  <si>
+    <t>Bank Taiwan Life 16</t>
+  </si>
+  <si>
+    <t>BNP Paribas Cardif TCB 14</t>
+  </si>
+  <si>
+    <t>BNP Paribas Cardif TCB 15</t>
+  </si>
+  <si>
+    <t>BNP Paribas Cardif TCB 16</t>
+  </si>
+  <si>
+    <t>Cardif 14</t>
+  </si>
+  <si>
+    <t>Cardif 15</t>
+  </si>
+  <si>
+    <t>Cardif 16</t>
+  </si>
+  <si>
+    <t>Cathay Life 14</t>
+  </si>
+  <si>
+    <t>Cathay Life 15</t>
+  </si>
+  <si>
+    <t>Cathay Life 16</t>
+  </si>
+  <si>
+    <t>DUMMY Cathay 15</t>
+  </si>
+  <si>
+    <t>Chaoyang Life 14</t>
+  </si>
+  <si>
+    <t>Chaoyang Life 15</t>
+  </si>
+  <si>
+    <t>Chaoyang Life 16</t>
+  </si>
+  <si>
+    <t>China Life 14</t>
+  </si>
+  <si>
+    <t>China Life 15</t>
+  </si>
+  <si>
+    <t>China Life 16</t>
+  </si>
+  <si>
+    <t>ACE Tempest Life 14</t>
+  </si>
+  <si>
+    <t>ACE Tempest Life 15</t>
+  </si>
+  <si>
+    <t>Chubb Tempest Life 16</t>
+  </si>
+  <si>
+    <t>Chunghwa Post 14</t>
+  </si>
+  <si>
+    <t>Chunghwa Post 15</t>
+  </si>
+  <si>
+    <t>Chunghwa Post 16</t>
+  </si>
+  <si>
+    <t>CIGNA 14</t>
+  </si>
+  <si>
+    <t>CIGNA 15</t>
+  </si>
+  <si>
+    <t>CIGNA 16</t>
+  </si>
+  <si>
+    <t>CTBC Life 14</t>
+  </si>
+  <si>
+    <t>CTBC Life 15</t>
+  </si>
+  <si>
+    <t>Farglory Life 14</t>
+  </si>
+  <si>
+    <t>Farglory Life 15</t>
+  </si>
+  <si>
+    <t>Farglory Life 16</t>
+  </si>
+  <si>
+    <t>First-Aviva Life 14</t>
+  </si>
+  <si>
+    <t>First-Aviva Life 15</t>
+  </si>
+  <si>
+    <t>First-Aviva Life 16</t>
+  </si>
+  <si>
+    <t>Fubon Life 14</t>
+  </si>
+  <si>
+    <t>Fubon Life 15</t>
+  </si>
+  <si>
+    <t>Fubon Life 16</t>
+  </si>
+  <si>
+    <t>Global Life 14</t>
+  </si>
+  <si>
+    <t>Hontai Life 14</t>
+  </si>
+  <si>
+    <t>Hontai Life 15</t>
+  </si>
+  <si>
+    <t>Hontai Life 16</t>
+  </si>
+  <si>
+    <t>Mercuries Life 14</t>
+  </si>
+  <si>
+    <t>Mercuries Life 15</t>
+  </si>
+  <si>
+    <t>Mercuries Life 16</t>
+  </si>
+  <si>
+    <t>Nan Shan Life 14</t>
+  </si>
+  <si>
+    <t>Nan Shan Life 15</t>
+  </si>
+  <si>
+    <t>Nan Shan Life 16</t>
+  </si>
+  <si>
+    <t>PCA Life 14</t>
+  </si>
+  <si>
+    <t>PCA Life 15</t>
+  </si>
+  <si>
+    <t>PCA Life 16</t>
+  </si>
+  <si>
+    <t>Prudential of Taiwan 14</t>
+  </si>
+  <si>
+    <t>Prudential of Taiwan 15</t>
+  </si>
+  <si>
+    <t>Prudential of Taiwan 16</t>
+  </si>
+  <si>
+    <t>Singfor Life 14</t>
+  </si>
+  <si>
+    <t>Shin Kong Life 14</t>
+  </si>
+  <si>
+    <t>Shin Kong Life 15</t>
+  </si>
+  <si>
+    <t>Shin Kong Life 16</t>
+  </si>
+  <si>
+    <t>Taiwan Life 14</t>
+  </si>
+  <si>
+    <t>Taiwan Life 15</t>
+  </si>
+  <si>
+    <t>Taiwan Life 16</t>
+  </si>
+  <si>
+    <t>DUMMY Taiwan 16</t>
+  </si>
+  <si>
+    <t>TransGlobe Life 14</t>
+  </si>
+  <si>
+    <t>TransGlobe Life 15</t>
+  </si>
+  <si>
+    <t>Yuanta Life 14</t>
+  </si>
+  <si>
+    <t>Yuanta Life 15</t>
+  </si>
+  <si>
+    <t>Yuanta Life 16</t>
+  </si>
+  <si>
+    <t>Zurich 14</t>
+  </si>
+  <si>
+    <t>Zurich 15</t>
+  </si>
+  <si>
+    <t>Zurich 16</t>
+  </si>
+  <si>
+    <t>[-0.1404  0.8596]</t>
+  </si>
+  <si>
+    <t>[0.7966 0.2034]</t>
+  </si>
+  <si>
+    <t>[-0.3835 -0.6165]</t>
+  </si>
+  <si>
+    <t>[-0.9343  0.0657]</t>
+  </si>
+  <si>
+    <t>[0.6572 0.3428]</t>
+  </si>
+  <si>
+    <t>[-0.5158  0.4842]</t>
+  </si>
+  <si>
+    <t>[ 0.0408 -0.9592]</t>
+  </si>
+  <si>
+    <t>[-0.0197 -0.9803]</t>
+  </si>
+  <si>
+    <t>[ 0.5945 -0.4055]</t>
+  </si>
+  <si>
+    <t>[0.7241 0.2759]</t>
+  </si>
+  <si>
+    <t>[ 0.4327 -0.5673]</t>
+  </si>
+  <si>
+    <t>[-0.5541 -0.4459]</t>
+  </si>
+  <si>
+    <t>[0.8918 0.1082]</t>
+  </si>
+  <si>
+    <t>[ 0.984 -0.016]</t>
+  </si>
+  <si>
+    <t>[-0.4484  0.5516]</t>
+  </si>
+  <si>
+    <t>[-0.2203  0.7797]</t>
+  </si>
+  <si>
+    <t>[-0.742  0.258]</t>
+  </si>
+  <si>
+    <t>[ 0.5208 -0.4792]</t>
+  </si>
+  <si>
+    <t>[ 0.4566 -0.5434]</t>
+  </si>
+  <si>
+    <t>[-0.1079 -0.8921]</t>
+  </si>
+  <si>
+    <t>[ 0.2064 -0.7936]</t>
+  </si>
+  <si>
+    <t>[-0.4433  0.5567]</t>
+  </si>
+  <si>
+    <t>[-0.351  0.649]</t>
+  </si>
+  <si>
+    <t>[ 0.5726 -0.4274]</t>
+  </si>
+  <si>
+    <t>[ 0.4369 -0.5631]</t>
+  </si>
+  <si>
+    <t>[0.7654 0.2346]</t>
+  </si>
+  <si>
+    <t>[-0.891 -0.109]</t>
+  </si>
+  <si>
+    <t>[-0.5038  0.4962]</t>
+  </si>
+  <si>
+    <t>[ 0.5464 -0.4536]</t>
+  </si>
+  <si>
+    <t>[0.0345 0.9655]</t>
+  </si>
+  <si>
+    <t>[ 0.5031 -0.4969]</t>
+  </si>
+  <si>
+    <t>[0.8986 0.1014]</t>
+  </si>
+  <si>
+    <t>[-0.9234  0.0766]</t>
+  </si>
+  <si>
+    <t>[-0.48  0.52]</t>
+  </si>
+  <si>
+    <t>[-0.4455  0.5545]</t>
+  </si>
+  <si>
+    <t>[ 0.6218 -0.3782]</t>
+  </si>
+  <si>
+    <t>[-0.6565  0.3435]</t>
+  </si>
+  <si>
+    <t>[-0.6686 -0.3314]</t>
+  </si>
+  <si>
+    <t>[ 0.4925 -0.5075]</t>
+  </si>
+  <si>
+    <t>[ 0.1742 -0.8258]</t>
+  </si>
+  <si>
+    <t>[-0.7532  0.2468]</t>
+  </si>
+  <si>
+    <t>[-0.3841  0.6159]</t>
+  </si>
+  <si>
+    <t>[-0.3817  0.6183]</t>
+  </si>
+  <si>
+    <t>[-0.6978 -0.3022]</t>
+  </si>
+  <si>
+    <t>[ 0.4241 -0.5759]</t>
+  </si>
+  <si>
+    <t>[-0.3637  0.6363]</t>
+  </si>
+  <si>
+    <t>[-0.4016  0.5984]</t>
+  </si>
+  <si>
+    <t>[-0.6043  0.3957]</t>
+  </si>
+  <si>
+    <t>[-0.4405  0.5595]</t>
+  </si>
+  <si>
+    <t>[-0.4123  0.5877]</t>
+  </si>
+  <si>
+    <t>[-0.5504  0.4496]</t>
+  </si>
+  <si>
+    <t>[-0.435  0.565]</t>
+  </si>
+  <si>
+    <t>[-0.44  0.56]</t>
+  </si>
+  <si>
+    <t>[-0.4598  0.5402]</t>
+  </si>
+  <si>
+    <t>[ 0.4459 -0.5541]</t>
+  </si>
+  <si>
+    <t>[ 0.4509 -0.5491]</t>
+  </si>
+  <si>
+    <t>[-0.4496  0.5504]</t>
+  </si>
+  <si>
+    <t>[ 0.4923 -0.5077]</t>
+  </si>
+  <si>
+    <t>[-0.5263  0.4737]</t>
+  </si>
+  <si>
+    <t>[-0.392  0.608]</t>
+  </si>
+  <si>
+    <t>[-0.0474 -0.9526]</t>
+  </si>
+  <si>
+    <t>[-0.4859  0.5141]</t>
+  </si>
+  <si>
+    <t>[ 0.4076 -0.5924]</t>
+  </si>
+  <si>
+    <t>[-0.5314  0.4686]</t>
+  </si>
+  <si>
+    <t>[ 0.5117 -0.4883]</t>
+  </si>
+  <si>
+    <t>[-0.3828 -0.6172]</t>
+  </si>
+  <si>
+    <t>[-0.4374  0.5626]</t>
+  </si>
+  <si>
+    <t>[ 0.4006 -0.5994]</t>
+  </si>
+  <si>
+    <t>[ 0.5247 -0.4753]</t>
+  </si>
+  <si>
+    <t>[-0.2897  0.7103]</t>
+  </si>
+  <si>
+    <t>[-0.9356 -0.0644]</t>
+  </si>
+  <si>
+    <t>[ 0.4762 -0.5238]</t>
+  </si>
+  <si>
+    <t>[-0.8277  0.1723]</t>
+  </si>
+  <si>
+    <t>[0.6924 0.3076]</t>
+  </si>
+  <si>
+    <t>[ 0.5541 -0.4459]</t>
+  </si>
+  <si>
+    <t>[ 9.991e-01 -9.000e-04]</t>
+  </si>
+  <si>
+    <t>[ 0.9922 -0.0078]</t>
+  </si>
+  <si>
+    <t>[nan nan]</t>
+  </si>
+  <si>
+    <t>[0 1]</t>
+  </si>
+  <si>
+    <t>[0 0]</t>
+  </si>
+  <si>
+    <t>[1 0]</t>
+  </si>
+  <si>
+    <t>TransGlobe Life 16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Marginal Profit Consistency</t>
-  </si>
-  <si>
-    <t>Efficiency</t>
-  </si>
-  <si>
-    <t>Efficiency Change</t>
-  </si>
-  <si>
-    <t>Scale</t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>AIA Taiwan 14</t>
-  </si>
-  <si>
-    <t>AIA Taiwan 15</t>
-  </si>
-  <si>
-    <t>AIA Taiwan 16</t>
-  </si>
-  <si>
-    <t>Allianz Taiwan Life 14</t>
-  </si>
-  <si>
-    <t>Allianz Taiwan Life 15</t>
-  </si>
-  <si>
-    <t>Allianz Taiwan Life 16</t>
-  </si>
-  <si>
-    <t>Bank Taiwan Life 14</t>
-  </si>
-  <si>
-    <t>Bank Taiwan Life 15</t>
-  </si>
-  <si>
-    <t>Bank Taiwan Life 16</t>
-  </si>
-  <si>
-    <t>BNP Paribas Cardif TCB 14</t>
-  </si>
-  <si>
-    <t>BNP Paribas Cardif TCB 15</t>
-  </si>
-  <si>
-    <t>BNP Paribas Cardif TCB 16</t>
-  </si>
-  <si>
-    <t>Cardif 14</t>
-  </si>
-  <si>
-    <t>Cardif 15</t>
-  </si>
-  <si>
-    <t>Cardif 16</t>
-  </si>
-  <si>
-    <t>Cathay Life 14</t>
-  </si>
-  <si>
-    <t>Cathay Life 15</t>
-  </si>
-  <si>
-    <t>Cathay Life 16</t>
-  </si>
-  <si>
-    <t>DUMMY Cathay 15</t>
-  </si>
-  <si>
-    <t>Chaoyang Life 14</t>
-  </si>
-  <si>
-    <t>Chaoyang Life 15</t>
-  </si>
-  <si>
-    <t>Chaoyang Life 16</t>
-  </si>
-  <si>
-    <t>China Life 14</t>
-  </si>
-  <si>
-    <t>China Life 15</t>
-  </si>
-  <si>
-    <t>China Life 16</t>
-  </si>
-  <si>
-    <t>ACE Tempest Life 14</t>
-  </si>
-  <si>
-    <t>ACE Tempest Life 15</t>
-  </si>
-  <si>
-    <t>Chubb Tempest Life 16</t>
-  </si>
-  <si>
-    <t>Chunghwa Post 14</t>
-  </si>
-  <si>
-    <t>Chunghwa Post 15</t>
-  </si>
-  <si>
-    <t>Chunghwa Post 16</t>
-  </si>
-  <si>
-    <t>CIGNA 14</t>
-  </si>
-  <si>
-    <t>CIGNA 15</t>
-  </si>
-  <si>
-    <t>CIGNA 16</t>
-  </si>
-  <si>
-    <t>CTBC Life 14</t>
-  </si>
-  <si>
-    <t>CTBC Life 15</t>
-  </si>
-  <si>
-    <t>Farglory Life 14</t>
-  </si>
-  <si>
-    <t>Farglory Life 15</t>
-  </si>
-  <si>
-    <t>Farglory Life 16</t>
-  </si>
-  <si>
-    <t>First-Aviva Life 14</t>
-  </si>
-  <si>
-    <t>First-Aviva Life 15</t>
-  </si>
-  <si>
-    <t>First-Aviva Life 16</t>
-  </si>
-  <si>
-    <t>Fubon Life 14</t>
-  </si>
-  <si>
-    <t>Fubon Life 15</t>
-  </si>
-  <si>
-    <t>Fubon Life 16</t>
-  </si>
-  <si>
-    <t>Global Life 14</t>
-  </si>
-  <si>
-    <t>Hontai Life 14</t>
-  </si>
-  <si>
-    <t>Hontai Life 15</t>
-  </si>
-  <si>
-    <t>Hontai Life 16</t>
-  </si>
-  <si>
-    <t>Mercuries Life 14</t>
-  </si>
-  <si>
-    <t>Mercuries Life 15</t>
-  </si>
-  <si>
-    <t>Mercuries Life 16</t>
-  </si>
-  <si>
-    <t>Nan Shan Life 14</t>
-  </si>
-  <si>
-    <t>Nan Shan Life 15</t>
-  </si>
-  <si>
-    <t>Nan Shan Life 16</t>
-  </si>
-  <si>
-    <t>PCA Life 14</t>
-  </si>
-  <si>
-    <t>PCA Life 15</t>
-  </si>
-  <si>
-    <t>PCA Life 16</t>
-  </si>
-  <si>
-    <t>Prudential of Taiwan 14</t>
-  </si>
-  <si>
-    <t>Prudential of Taiwan 15</t>
-  </si>
-  <si>
-    <t>Prudential of Taiwan 16</t>
-  </si>
-  <si>
-    <t>Singfor Life 14</t>
-  </si>
-  <si>
-    <t>Shin Kong Life 14</t>
-  </si>
-  <si>
-    <t>Shin Kong Life 15</t>
-  </si>
-  <si>
-    <t>Shin Kong Life 16</t>
-  </si>
-  <si>
-    <t>Taiwan Life 14</t>
-  </si>
-  <si>
-    <t>Taiwan Life 15</t>
-  </si>
-  <si>
-    <t>Taiwan Life 16</t>
-  </si>
-  <si>
-    <t>DUMMY Taiwan 16</t>
-  </si>
-  <si>
-    <t>TransGlobe Life 14</t>
-  </si>
-  <si>
-    <t>TransGlobe Life 15</t>
-  </si>
-  <si>
-    <t>TransGlobe Life 16</t>
-  </si>
-  <si>
-    <t>Yuanta Life 14</t>
-  </si>
-  <si>
-    <t>Yuanta Life 15</t>
-  </si>
-  <si>
-    <t>Yuanta Life 16</t>
-  </si>
-  <si>
-    <t>Zurich 14</t>
-  </si>
-  <si>
-    <t>Zurich 15</t>
-  </si>
-  <si>
-    <t>Zurich 16</t>
-  </si>
-  <si>
-    <t>[-0.1404  0.8596]</t>
-  </si>
-  <si>
-    <t>[0.7966 0.2034]</t>
-  </si>
-  <si>
-    <t>[-0.3835 -0.6165]</t>
-  </si>
-  <si>
-    <t>[-0.9343  0.0657]</t>
-  </si>
-  <si>
-    <t>[0.6572 0.3428]</t>
-  </si>
-  <si>
-    <t>[-0.5158  0.4842]</t>
-  </si>
-  <si>
-    <t>[ 0.0408 -0.9592]</t>
-  </si>
-  <si>
-    <t>[-0.0197 -0.9803]</t>
-  </si>
-  <si>
-    <t>[ 0.5945 -0.4055]</t>
-  </si>
-  <si>
-    <t>[0.7241 0.2759]</t>
-  </si>
-  <si>
-    <t>[ 0.4327 -0.5673]</t>
-  </si>
-  <si>
-    <t>[-0.5541 -0.4459]</t>
-  </si>
-  <si>
-    <t>[0.8918 0.1082]</t>
-  </si>
-  <si>
-    <t>[ 0.984 -0.016]</t>
-  </si>
-  <si>
-    <t>[-0.4484  0.5516]</t>
-  </si>
-  <si>
-    <t>[-0.2203  0.7797]</t>
-  </si>
-  <si>
-    <t>[-0.742  0.258]</t>
-  </si>
-  <si>
-    <t>[ 0.5208 -0.4792]</t>
-  </si>
-  <si>
-    <t>[ 0.4566 -0.5434]</t>
-  </si>
-  <si>
-    <t>[-0.1079 -0.8921]</t>
-  </si>
-  <si>
-    <t>[ 0.2064 -0.7936]</t>
-  </si>
-  <si>
-    <t>[-0.4433  0.5567]</t>
-  </si>
-  <si>
-    <t>[-0.351  0.649]</t>
-  </si>
-  <si>
-    <t>[ 0.5726 -0.4274]</t>
-  </si>
-  <si>
-    <t>[ 0.4369 -0.5631]</t>
-  </si>
-  <si>
-    <t>[0.7654 0.2346]</t>
-  </si>
-  <si>
-    <t>[-0.891 -0.109]</t>
-  </si>
-  <si>
-    <t>[-0.5038  0.4962]</t>
-  </si>
-  <si>
-    <t>[ 0.5464 -0.4536]</t>
-  </si>
-  <si>
-    <t>[0.0345 0.9655]</t>
-  </si>
-  <si>
-    <t>[ 0.5031 -0.4969]</t>
-  </si>
-  <si>
-    <t>[0.8986 0.1014]</t>
-  </si>
-  <si>
-    <t>[-0.9234  0.0766]</t>
-  </si>
-  <si>
-    <t>[-0.48  0.52]</t>
-  </si>
-  <si>
-    <t>[-0.4455  0.5545]</t>
-  </si>
-  <si>
-    <t>[ 0.6218 -0.3782]</t>
-  </si>
-  <si>
-    <t>[-0.6565  0.3435]</t>
-  </si>
-  <si>
-    <t>[-0.6686 -0.3314]</t>
-  </si>
-  <si>
-    <t>[ 0.4925 -0.5075]</t>
-  </si>
-  <si>
-    <t>[ 0.1742 -0.8258]</t>
-  </si>
-  <si>
-    <t>[-0.7532  0.2468]</t>
-  </si>
-  <si>
-    <t>[-0.3841  0.6159]</t>
-  </si>
-  <si>
-    <t>[-0.3817  0.6183]</t>
-  </si>
-  <si>
-    <t>[-0.6978 -0.3022]</t>
-  </si>
-  <si>
-    <t>[ 0.4241 -0.5759]</t>
-  </si>
-  <si>
-    <t>[-0.3637  0.6363]</t>
-  </si>
-  <si>
-    <t>[-0.4016  0.5984]</t>
-  </si>
-  <si>
-    <t>[-0.6043  0.3957]</t>
-  </si>
-  <si>
-    <t>[-0.4405  0.5595]</t>
-  </si>
-  <si>
-    <t>[-0.4123  0.5877]</t>
-  </si>
-  <si>
-    <t>[-0.5504  0.4496]</t>
-  </si>
-  <si>
-    <t>[-0.435  0.565]</t>
-  </si>
-  <si>
-    <t>[-0.44  0.56]</t>
-  </si>
-  <si>
-    <t>[-0.4598  0.5402]</t>
-  </si>
-  <si>
-    <t>[ 0.4459 -0.5541]</t>
-  </si>
-  <si>
-    <t>[ 0.4509 -0.5491]</t>
-  </si>
-  <si>
-    <t>[-0.4496  0.5504]</t>
-  </si>
-  <si>
-    <t>[ 0.4923 -0.5077]</t>
-  </si>
-  <si>
-    <t>[-0.5263  0.4737]</t>
-  </si>
-  <si>
-    <t>[-0.392  0.608]</t>
-  </si>
-  <si>
-    <t>[-0.0474 -0.9526]</t>
-  </si>
-  <si>
-    <t>[-0.4859  0.5141]</t>
-  </si>
-  <si>
-    <t>[ 0.4076 -0.5924]</t>
-  </si>
-  <si>
-    <t>[-0.5314  0.4686]</t>
-  </si>
-  <si>
-    <t>[ 0.5117 -0.4883]</t>
-  </si>
-  <si>
-    <t>[-0.3828 -0.6172]</t>
-  </si>
-  <si>
-    <t>[-0.4374  0.5626]</t>
-  </si>
-  <si>
-    <t>[ 0.4006 -0.5994]</t>
-  </si>
-  <si>
-    <t>[ 0.5247 -0.4753]</t>
-  </si>
-  <si>
-    <t>[-0.2897  0.7103]</t>
-  </si>
-  <si>
-    <t>[-0.9356 -0.0644]</t>
-  </si>
-  <si>
-    <t>[ 0.4762 -0.5238]</t>
-  </si>
-  <si>
-    <t>[-0.8277  0.1723]</t>
-  </si>
-  <si>
-    <t>[0.6924 0.3076]</t>
-  </si>
-  <si>
-    <t>[ 0.5541 -0.4459]</t>
-  </si>
-  <si>
-    <t>[ 9.991e-01 -9.000e-04]</t>
-  </si>
-  <si>
-    <t>[ 0.9922 -0.0078]</t>
-  </si>
-  <si>
-    <t>[nan nan]</t>
-  </si>
-  <si>
-    <t>[0 1]</t>
-  </si>
-  <si>
-    <t>[0 0]</t>
-  </si>
-  <si>
-    <t>[1 0]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -972,7 +974,8 @@
   <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1021,24 +1024,24 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3">
         <v>1.0019</v>
@@ -1053,22 +1056,22 @@
         <v>1.7022999999999999</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" s="3">
         <v>0.5363</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J2" s="4">
         <v>0.9869</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L2" s="4">
         <v>0</v>
@@ -1091,7 +1094,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
         <v>0.93769999999999998</v>
@@ -1106,22 +1109,22 @@
         <v>1.9300999999999999</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="3">
         <v>0.58340000000000003</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J3" s="4">
         <v>0.24740000000000001</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L3" s="4">
         <v>0</v>
@@ -1144,7 +1147,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3">
         <v>0.87809999999999999</v>
@@ -1159,22 +1162,22 @@
         <v>2.0322</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="3">
         <v>0.63129999999999997</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J4" s="4">
         <v>-0.84909999999999997</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L4" s="4">
         <v>0</v>
@@ -1197,7 +1200,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>3.1435</v>
@@ -1212,22 +1215,22 @@
         <v>1.7201</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5">
         <v>0.78749999999999998</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J5" s="5">
         <v>0</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L5" s="5">
         <v>0</v>
@@ -1250,7 +1253,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>4.5007999999999999</v>
@@ -1265,22 +1268,22 @@
         <v>1.8231999999999999</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6">
         <v>0.99429999999999996</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J6" s="5">
         <v>0</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L6" s="5">
         <v>0</v>
@@ -1303,7 +1306,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>3.6065</v>
@@ -1318,22 +1321,22 @@
         <v>2.3632</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7">
         <v>0.92130000000000001</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J7" s="5">
         <v>0</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L7" s="5">
         <v>0</v>
@@ -1356,7 +1359,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3">
         <v>1.8587</v>
@@ -1371,22 +1374,22 @@
         <v>12.176500000000001</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="3">
         <v>0.6552</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J8" s="4">
         <v>0</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L8" s="4">
         <v>4.2500000000000003E-2</v>
@@ -1409,7 +1412,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>2.3653</v>
@@ -1424,22 +1427,22 @@
         <v>10.387</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="3">
         <v>0.93989999999999996</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J9" s="4">
         <v>0</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L9" s="4">
         <v>-0.99980000000000002</v>
@@ -1462,7 +1465,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3">
         <v>2.9632000000000001</v>
@@ -1477,22 +1480,22 @@
         <v>9.7167999999999992</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="3">
         <v>0.92679999999999996</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J10" s="4">
         <v>0</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L10" s="4">
         <v>-0.56340000000000001</v>
@@ -1515,7 +1518,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>1.0458000000000001</v>
@@ -1530,22 +1533,22 @@
         <v>2.0626000000000002</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H11">
         <v>0.72629999999999995</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J11" s="5">
         <v>0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L11" s="5">
         <v>0</v>
@@ -1568,7 +1571,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>1.3233999999999999</v>
@@ -1583,22 +1586,22 @@
         <v>2.1907999999999999</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H12">
         <v>0.66459999999999997</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J12" s="5">
         <v>0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L12" s="5">
         <v>0</v>
@@ -1621,7 +1624,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>1.1358999999999999</v>
@@ -1636,22 +1639,22 @@
         <v>1.8709</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H13">
         <v>0.63</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J13" s="5">
         <v>0</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L13" s="5">
         <v>0</v>
@@ -1674,7 +1677,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3">
         <v>4.6574999999999998</v>
@@ -1689,22 +1692,22 @@
         <v>1.04</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J14" s="4">
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L14" s="4">
         <v>0</v>
@@ -1727,7 +1730,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3">
         <v>4.7965</v>
@@ -1742,22 +1745,22 @@
         <v>1.1474</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="3">
         <v>0.99970000000000003</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J15" s="4">
         <v>0</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L15" s="4">
         <v>0</v>
@@ -1780,7 +1783,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3">
         <v>3.5586000000000002</v>
@@ -1795,22 +1798,22 @@
         <v>1.121</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L16" s="4">
         <v>0</v>
@@ -1833,7 +1836,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>32.2151</v>
@@ -1848,22 +1851,22 @@
         <v>169.2475</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L17" s="5">
         <v>-0.27189999999999998</v>
@@ -1886,7 +1889,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>32.787799999999997</v>
@@ -1901,22 +1904,22 @@
         <v>182.49760000000001</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J18" s="5">
         <v>0</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L18" s="5">
         <v>0</v>
@@ -1939,7 +1942,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>37.923999999999999</v>
@@ -1954,22 +1957,22 @@
         <v>191.2397</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J19" s="5">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L19" s="5">
         <v>0</v>
@@ -1992,7 +1995,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>33.6128</v>
@@ -2007,22 +2010,22 @@
         <v>171.89519999999999</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J20" s="5">
         <v>0</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L20" s="5">
         <v>0.64329999999999998</v>
@@ -2045,7 +2048,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3">
         <v>0.80249999999999999</v>
@@ -2060,22 +2063,22 @@
         <v>3.1263000000000001</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J21" s="4">
         <v>0</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L21" s="4">
         <v>-0.99280000000000002</v>
@@ -2098,7 +2101,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3">
         <v>0.76619999999999999</v>
@@ -2113,22 +2116,22 @@
         <v>1.7727999999999999</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H22" s="3">
         <v>0.88660000000000005</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J22" s="4">
         <v>0</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L22" s="4">
         <v>0</v>
@@ -2151,7 +2154,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3">
         <v>0.71430000000000005</v>
@@ -2166,22 +2169,22 @@
         <v>1.5447</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H23" s="3">
         <v>0.8679</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J23" s="4">
         <v>0</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L23" s="4">
         <v>0</v>
@@ -2204,7 +2207,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>9.5121000000000002</v>
@@ -2219,22 +2222,22 @@
         <v>39.691499999999998</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24">
         <v>0.76100000000000001</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J24" s="5">
         <v>-0.47560000000000002</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L24" s="5">
         <v>-0.47560000000000002</v>
@@ -2257,7 +2260,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>13.5952</v>
@@ -2272,22 +2275,22 @@
         <v>47.904899999999998</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J25" s="5">
         <v>0</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L25" s="5">
         <v>0.8014</v>
@@ -2310,7 +2313,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>11.731</v>
@@ -2325,22 +2328,22 @@
         <v>47.708599999999997</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J26" s="5">
         <v>0.61309999999999998</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L26" s="5">
         <v>0.61309999999999998</v>
@@ -2363,7 +2366,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="3">
         <v>0.85529999999999995</v>
@@ -2378,22 +2381,22 @@
         <v>0.76980000000000004</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H27" s="3">
         <v>0.6905</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J27" s="4">
         <v>0</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L27" s="4">
         <v>0</v>
@@ -2416,7 +2419,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3">
         <v>0.82289999999999996</v>
@@ -2431,22 +2434,22 @@
         <v>0.79679999999999995</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H28" s="3">
         <v>0.61180000000000001</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J28" s="4">
         <v>0</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L28" s="4">
         <v>0</v>
@@ -2469,7 +2472,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="3">
         <v>1.0187999999999999</v>
@@ -2484,22 +2487,22 @@
         <v>0.7722</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H29" s="3">
         <v>0.55800000000000005</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J29" s="4">
         <v>0</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L29" s="4">
         <v>0</v>
@@ -2522,7 +2525,7 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>0.4869</v>
@@ -2537,22 +2540,22 @@
         <v>20.221399999999999</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J30" s="5">
         <v>0.76939999999999997</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L30" s="5">
         <v>0</v>
@@ -2575,7 +2578,7 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>0.376</v>
@@ -2590,22 +2593,22 @@
         <v>19.016100000000002</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J31" s="5">
         <v>3.5799999999999998E-2</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L31" s="5">
         <v>0</v>
@@ -2628,7 +2631,7 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>0.52800000000000002</v>
@@ -2643,22 +2646,22 @@
         <v>19.298999999999999</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J32" s="5">
         <v>0.71150000000000002</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L32" s="5">
         <v>0.71150000000000002</v>
@@ -2681,7 +2684,7 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="3">
         <v>1.1580999999999999</v>
@@ -2696,22 +2699,22 @@
         <v>0.93479999999999996</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H33" s="3">
         <v>0.94299999999999995</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J33" s="4">
         <v>0.11219999999999999</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L33" s="4">
         <v>0</v>
@@ -2734,7 +2737,7 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3">
         <v>1.0128999999999999</v>
@@ -2749,22 +2752,22 @@
         <v>0.97299999999999998</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H34" s="3">
         <v>1</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J34" s="4">
         <v>8.2600000000000007E-2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L34" s="4">
         <v>0</v>
@@ -2787,7 +2790,7 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="3">
         <v>0.90800000000000003</v>
@@ -2802,22 +2805,22 @@
         <v>1.0101</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H35" s="3">
         <v>0.88370000000000004</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J35" s="4">
         <v>0.73480000000000001</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L35" s="4">
         <v>0</v>
@@ -2840,7 +2843,7 @@
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36">
         <v>10.8484</v>
@@ -2855,22 +2858,22 @@
         <v>12.6541</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H36">
         <v>0.61350000000000005</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J36" s="5">
         <v>0</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L36" s="5">
         <v>0</v>
@@ -2893,7 +2896,7 @@
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37">
         <v>10.632</v>
@@ -2908,22 +2911,22 @@
         <v>16.4587</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H37">
         <v>0.61580000000000001</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J37" s="5">
         <v>0</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L37" s="5">
         <v>0</v>
@@ -2946,7 +2949,7 @@
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="3">
         <v>3.6964999999999999</v>
@@ -2961,22 +2964,22 @@
         <v>13.583</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H38" s="3">
         <v>0.82630000000000003</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J38" s="4">
         <v>0</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L38" s="4">
         <v>0</v>
@@ -2999,7 +3002,7 @@
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="3">
         <v>4.8190999999999997</v>
@@ -3014,22 +3017,22 @@
         <v>14.106999999999999</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H39" s="3">
         <v>0.4844</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J39" s="4">
         <v>0</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L39" s="4">
         <v>0</v>
@@ -3052,7 +3055,7 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="3">
         <v>7.2412000000000001</v>
@@ -3067,22 +3070,22 @@
         <v>13.058199999999999</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H40" s="3">
         <v>0.54679999999999995</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J40" s="4">
         <v>0</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L40" s="4">
         <v>0</v>
@@ -3105,7 +3108,7 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41">
         <v>0.6139</v>
@@ -3120,22 +3123,22 @@
         <v>1.0580000000000001</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H41">
         <v>0.78449999999999998</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J41" s="5">
         <v>0</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L41" s="5">
         <v>0</v>
@@ -3158,7 +3161,7 @@
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42">
         <v>0.67989999999999995</v>
@@ -3173,22 +3176,22 @@
         <v>0.96379999999999999</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H42">
         <v>0.73319999999999996</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J42" s="5">
         <v>0</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L42" s="5">
         <v>0</v>
@@ -3211,7 +3214,7 @@
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43">
         <v>0.57589999999999997</v>
@@ -3226,22 +3229,22 @@
         <v>0.99350000000000005</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H43">
         <v>0.74590000000000001</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J43" s="5">
         <v>0</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L43" s="5">
         <v>0</v>
@@ -3264,7 +3267,7 @@
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="3">
         <v>23.229500000000002</v>
@@ -3279,22 +3282,22 @@
         <v>110.49720000000001</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H44" s="3">
         <v>0.84540000000000004</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J44" s="4">
         <v>0</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L44" s="4">
         <v>0</v>
@@ -3317,7 +3320,7 @@
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="3">
         <v>26.095700000000001</v>
@@ -3332,22 +3335,22 @@
         <v>130.68</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H45" s="3">
         <v>1</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J45" s="4">
         <v>0</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L45" s="4">
         <v>0</v>
@@ -3370,7 +3373,7 @@
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="3">
         <v>33.474600000000002</v>
@@ -3385,22 +3388,22 @@
         <v>124.6546</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H46" s="3">
         <v>0.87870000000000004</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J46" s="4">
         <v>0</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L46" s="4">
         <v>0</v>
@@ -3423,7 +3426,7 @@
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47">
         <v>0.89319999999999999</v>
@@ -3438,22 +3441,22 @@
         <v>2.2202000000000002</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H47">
         <v>0.81430000000000002</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J47" s="5">
         <v>0</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L47" s="5">
         <v>0</v>
@@ -3476,7 +3479,7 @@
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3">
         <v>0.79630000000000001</v>
@@ -3491,22 +3494,22 @@
         <v>7.8590999999999998</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H48" s="3">
         <v>0.78249999999999997</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J48" s="4">
         <v>0</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L48" s="4">
         <v>-0.55730000000000002</v>
@@ -3529,7 +3532,7 @@
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3">
         <v>0.69620000000000004</v>
@@ -3544,22 +3547,22 @@
         <v>8.5192999999999994</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H49" s="3">
         <v>1</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J49" s="4">
         <v>0</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L49" s="4">
         <v>-0.83660000000000001</v>
@@ -3582,7 +3585,7 @@
     </row>
     <row r="50" spans="1:17">
       <c r="A50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="3">
         <v>0.8196</v>
@@ -3597,22 +3600,22 @@
         <v>8.9616000000000007</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H50" s="3">
         <v>0.7419</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J50" s="4">
         <v>0</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L50" s="4">
         <v>-0.61860000000000004</v>
@@ -3635,7 +3638,7 @@
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51">
         <v>11.0647</v>
@@ -3650,22 +3653,22 @@
         <v>25.008099999999999</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H51">
         <v>0.80610000000000004</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J51" s="5">
         <v>0</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L51" s="5">
         <v>0</v>
@@ -3688,7 +3691,7 @@
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B52">
         <v>11.212199999999999</v>
@@ -3703,22 +3706,22 @@
         <v>28.885300000000001</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H52">
         <v>0.77429999999999999</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J52" s="5">
         <v>0</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L52" s="5">
         <v>0</v>
@@ -3741,7 +3744,7 @@
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53">
         <v>11.918699999999999</v>
@@ -3756,22 +3759,22 @@
         <v>31.266500000000001</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H53">
         <v>0.75270000000000004</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J53" s="5">
         <v>0</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L53" s="5">
         <v>0</v>
@@ -3794,7 +3797,7 @@
     </row>
     <row r="54" spans="1:17">
       <c r="A54" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" s="3">
         <v>18.230799999999999</v>
@@ -3809,22 +3812,22 @@
         <v>118.0595</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H54" s="3">
         <v>0.57899999999999996</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J54" s="4">
         <v>-0.61780000000000002</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L54" s="4">
         <v>0</v>
@@ -3847,7 +3850,7 @@
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B55" s="3">
         <v>19.526599999999998</v>
@@ -3862,22 +3865,22 @@
         <v>131.93170000000001</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H55" s="3">
         <v>0.72230000000000005</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J55" s="4">
         <v>-0.6482</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L55" s="4">
         <v>0</v>
@@ -3900,7 +3903,7 @@
     </row>
     <row r="56" spans="1:17">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B56" s="3">
         <v>21.436800000000002</v>
@@ -3915,22 +3918,22 @@
         <v>152.58080000000001</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H56" s="3">
         <v>1</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J56" s="4">
         <v>0.62690000000000001</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L56" s="4">
         <v>0</v>
@@ -3953,7 +3956,7 @@
     </row>
     <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57">
         <v>1.8171999999999999</v>
@@ -3968,22 +3971,22 @@
         <v>6.6342999999999996</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H57">
         <v>0.52010000000000001</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J57" s="5">
         <v>-0.77280000000000004</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L57" s="5">
         <v>0</v>
@@ -4006,7 +4009,7 @@
     </row>
     <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B58">
         <v>1.6254999999999999</v>
@@ -4021,22 +4024,22 @@
         <v>0</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H58">
         <v>0.75939999999999996</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J58" s="5">
         <v>0.77439999999999998</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L58" s="5">
         <v>0</v>
@@ -4059,7 +4062,7 @@
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>1.7653000000000001</v>
@@ -4074,22 +4077,22 @@
         <v>8.3163</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H59">
         <v>0.70960000000000001</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J59" s="5">
         <v>0</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L59" s="5">
         <v>0</v>
@@ -4112,7 +4115,7 @@
     </row>
     <row r="60" spans="1:17">
       <c r="A60" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" s="3">
         <v>0.86850000000000005</v>
@@ -4127,22 +4130,22 @@
         <v>3.4958999999999998</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H60" s="3">
         <v>0.65369999999999995</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J60" s="4">
         <v>0</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L60" s="4">
         <v>0</v>
@@ -4165,7 +4168,7 @@
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B61" s="3">
         <v>0.85389999999999999</v>
@@ -4180,22 +4183,22 @@
         <v>3.7054999999999998</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H61" s="3">
         <v>0.71079999999999999</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J61" s="4">
         <v>0</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L61" s="4">
         <v>0</v>
@@ -4218,7 +4221,7 @@
     </row>
     <row r="62" spans="1:17">
       <c r="A62" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" s="3">
         <v>0.98299999999999998</v>
@@ -4233,22 +4236,22 @@
         <v>4.6002000000000001</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H62" s="3">
         <v>0.75660000000000005</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J62" s="4">
         <v>0</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L62" s="4">
         <v>0</v>
@@ -4271,7 +4274,7 @@
     </row>
     <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B63">
         <v>0.50439999999999996</v>
@@ -4286,22 +4289,22 @@
         <v>1.9418</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H63">
         <v>0.77680000000000005</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J63" s="5">
         <v>0</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L63" s="5">
         <v>0</v>
@@ -4324,7 +4327,7 @@
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B64" s="3">
         <v>8.6320999999999994</v>
@@ -4339,22 +4342,22 @@
         <v>77.970699999999994</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H64" s="3">
         <v>1</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J64" s="4">
         <v>0.56689999999999996</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L64" s="4">
         <v>0</v>
@@ -4377,7 +4380,7 @@
     </row>
     <row r="65" spans="1:17">
       <c r="A65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="3">
         <v>7.9958999999999998</v>
@@ -4392,22 +4395,22 @@
         <v>71.694699999999997</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H65" s="3">
         <v>0.82199999999999995</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J65" s="4">
         <v>-0.75009999999999999</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L65" s="4">
         <v>0</v>
@@ -4430,7 +4433,7 @@
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="3">
         <v>13.287699999999999</v>
@@ -4445,22 +4448,22 @@
         <v>80.386300000000006</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H66" s="3">
         <v>0.43059999999999998</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J66" s="4">
         <v>0.72340000000000004</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L66" s="4">
         <v>0</v>
@@ -4483,7 +4486,7 @@
     </row>
     <row r="67" spans="1:17">
       <c r="A67" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67">
         <v>2.54</v>
@@ -4498,22 +4501,22 @@
         <v>18.720800000000001</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H67">
         <v>0.56740000000000002</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J67" s="5">
         <v>0</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L67" s="5">
         <v>0</v>
@@ -4536,7 +4539,7 @@
     </row>
     <row r="68" spans="1:17">
       <c r="A68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68">
         <v>2.3294999999999999</v>
@@ -4551,22 +4554,22 @@
         <v>16.5044</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H68">
         <v>0.62770000000000004</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J68" s="5">
         <v>0</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L68" s="5">
         <v>0</v>
@@ -4589,7 +4592,7 @@
     </row>
     <row r="69" spans="1:17">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69">
         <v>17.659400000000002</v>
@@ -4604,22 +4607,22 @@
         <v>44.705399999999997</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H69">
         <v>0.52059999999999995</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J69" s="5">
         <v>0</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L69" s="5">
         <v>0.55559999999999998</v>
@@ -4642,7 +4645,7 @@
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70">
         <v>12.961499999999999</v>
@@ -4657,22 +4660,22 @@
         <v>32.206000000000003</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H70">
         <v>0.74060000000000004</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J70" s="5">
         <v>0</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L70" s="5">
         <v>0</v>
@@ -4695,7 +4698,7 @@
     </row>
     <row r="71" spans="1:17">
       <c r="A71" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B71" s="3">
         <v>5.4183000000000003</v>
@@ -4710,22 +4713,22 @@
         <v>26.5852</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H71" s="3">
         <v>0.56510000000000005</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J71" s="4">
         <v>0</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L71" s="4">
         <v>0</v>
@@ -4748,7 +4751,7 @@
     </row>
     <row r="72" spans="1:17">
       <c r="A72" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" s="3">
         <v>5.1632999999999996</v>
@@ -4763,22 +4766,22 @@
         <v>34.042400000000001</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H72" s="3">
         <v>0.54730000000000001</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J72" s="4">
         <v>0</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L72" s="4">
         <v>-0.99760000000000004</v>
@@ -4801,7 +4804,7 @@
     </row>
     <row r="73" spans="1:17">
       <c r="A73" s="2" t="s">
-        <v>87</v>
+        <v>173</v>
       </c>
       <c r="B73" s="3">
         <v>6.4225000000000003</v>
@@ -4816,22 +4819,22 @@
         <v>33.824599999999997</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H73" s="3">
         <v>0.71730000000000005</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J73" s="4">
         <v>0</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L73" s="4">
         <v>0.67269999999999996</v>
@@ -4854,7 +4857,7 @@
     </row>
     <row r="74" spans="1:17">
       <c r="A74" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B74">
         <v>1.6259999999999999</v>
@@ -4869,22 +4872,22 @@
         <v>3.5472999999999999</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H74">
         <v>0.6028</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J74" s="5">
         <v>0</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L74" s="5">
         <v>0</v>
@@ -4907,7 +4910,7 @@
     </row>
     <row r="75" spans="1:17">
       <c r="A75" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B75">
         <v>4.7514000000000003</v>
@@ -4922,22 +4925,22 @@
         <v>4.1646000000000001</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H75">
         <v>0.7077</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J75" s="5">
         <v>0</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L75" s="5">
         <v>0</v>
@@ -4960,7 +4963,7 @@
     </row>
     <row r="76" spans="1:17">
       <c r="A76" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B76">
         <v>2.2856000000000001</v>
@@ -4975,22 +4978,22 @@
         <v>4.6909999999999998</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H76">
         <v>0.4546</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J76" s="5">
         <v>0</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L76" s="5">
         <v>0</v>
@@ -5013,7 +5016,7 @@
     </row>
     <row r="77" spans="1:17">
       <c r="A77" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B77" s="3">
         <v>7.7999999999999996E-3</v>
@@ -5028,22 +5031,22 @@
         <v>0.7581</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H77" s="3">
         <v>0.99280000000000002</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J77" s="4">
         <v>0</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L77" s="4">
         <v>0</v>
@@ -5066,7 +5069,7 @@
     </row>
     <row r="78" spans="1:17">
       <c r="A78" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B78" s="3">
         <v>2.3E-3</v>
@@ -5081,22 +5084,22 @@
         <v>0.7581</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H78" s="3">
         <v>0.99919999999999998</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J78" s="4">
         <v>0</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L78" s="4">
         <v>0</v>
@@ -5119,7 +5122,7 @@
     </row>
     <row r="79" spans="1:17">
       <c r="A79" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B79" s="3">
         <v>5.9999999999999995E-4</v>
@@ -5134,22 +5137,22 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H79" s="3">
         <v>1</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J79" s="4">
         <v>0</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L79" s="4">
         <v>0</v>

</xml_diff>